<commit_message>
Support OpenCSV pre-assignment validators and custom converters for Excel readers
</commit_message>
<xml_diff>
--- a/src/test/resources/sample.xlsx
+++ b/src/test/resources/sample.xlsx
@@ -65,7 +65,7 @@
     <t>伊藤美咲</t>
   </si>
   <si>
-    <t>札幌</t>
+    <t>横浜</t>
   </si>
 </sst>
 </file>
@@ -191,10 +191,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>27.0</v>
+        <v>22.0</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
feat: add ignoreQuotations option for CSV/TSV parsing
</commit_message>
<xml_diff>
--- a/src/test/resources/sample.xlsx
+++ b/src/test/resources/sample.xlsx
@@ -65,7 +65,7 @@
     <t>伊藤美咲</t>
   </si>
   <si>
-    <t>札幌</t>
+    <t>横浜</t>
   </si>
 </sst>
 </file>
@@ -191,10 +191,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>27.0</v>
+        <v>22.0</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>17</v>

</xml_diff>